<commit_message>
Second round of pre-CRAN fixes
</commit_message>
<xml_diff>
--- a/inst/DistrNames.xlsx
+++ b/inst/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\Gov2k1inSilico\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834E32FC-EA88-4978-81BE-1583BD42D5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF15F46-BEBE-4321-8CF8-FD536C7F9952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="166">
   <si>
     <t>Poisson</t>
   </si>
@@ -519,22 +519,19 @@
     <t>c(-1,.6,2, 1,.5,.25)</t>
   </si>
   <si>
+    <t>$ \tilde{E}(y) = \tilde{\pi} = \tilde{Pr}(Y=1)$</t>
+  </si>
+  <si>
+    <t>$ \tilde{E}(y) =\tilde{\pi} = \tilde{Pr}(Y=1)$</t>
+  </si>
+  <si>
     <t>$ \tilde{E}(y) =\tilde{\mu} = \bar{Y}$</t>
   </si>
   <si>
-    <t>$ \tilde{E}(y) = \tilde{\pi} = \tilde{Pr}(Y=1)$</t>
-  </si>
-  <si>
-    <t>$ \tilde{E}(y) =\tilde{\pi} = \tilde{Pr}(Y=1)$</t>
-  </si>
-  <si>
     <t>$ \tilde{E}(y)$</t>
   </si>
   <si>
     <t>$ \tilde{E}(y) =\tilde{\lambda} = \bar{Y}$</t>
-  </si>
-  <si>
-    <t>$blorg$</t>
   </si>
 </sst>
 </file>
@@ -903,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:AN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1091,7 +1088,7 @@
         <v>114</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>127</v>
@@ -1224,7 +1221,7 @@
         <v>113</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>129</v>
@@ -1357,7 +1354,7 @@
         <v>113</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>131</v>
@@ -1490,7 +1487,7 @@
         <v>113</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>131</v>
@@ -1623,7 +1620,7 @@
         <v>113</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>130</v>
@@ -1756,7 +1753,7 @@
         <v>113</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>130</v>
@@ -1889,7 +1886,7 @@
         <v>113</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>129</v>
@@ -2022,7 +2019,7 @@
         <v>113</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>131</v>
@@ -2155,7 +2152,7 @@
         <v>113</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>133</v>
@@ -2953,7 +2950,7 @@
         <v>113</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>132</v>

</xml_diff>